<commit_message>
feat: Add sample budget files and update main_backtest example for improved functionality
</commit_message>
<xml_diff>
--- a/data/orcamentos/sample_padrao2_japj.xlsx
+++ b/data/orcamentos/sample_padrao2_japj.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/orcamentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="80" documentId="11_2B596957557796436140C5F050CBC83569B5E5FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E39250D-D8F3-4996-9083-83386660E9D8}"/>
@@ -634,7 +634,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>